<commit_message>
New version of word, excel and powerpoint
</commit_message>
<xml_diff>
--- a/Proyecto.xlsx
+++ b/Proyecto.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paola Fajardo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paola Fajardo\Desktop\DOCUMENTOS INTEGRADOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200BA6A5-31A5-4DE9-85F7-ED05CEA2D3FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6DEE810-48CC-4896-AEE6-6F00E9681ABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{697E0B3F-7130-415E-993A-8AD87E12B9CD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{697E0B3F-7130-415E-993A-8AD87E12B9CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="7" r:id="rId1"/>
     <sheet name="Project" sheetId="2" r:id="rId2"/>
     <sheet name="Rubricas" sheetId="9" r:id="rId3"/>
     <sheet name="Tools" sheetId="8" r:id="rId4"/>
-    <sheet name="Refe" sheetId="6" r:id="rId5"/>
+    <sheet name="Refe" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_Estructura">#N/A</definedName>
@@ -26,6 +26,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="97">
   <si>
     <t>Task</t>
   </si>
@@ -348,6 +349,9 @@
   <si>
     <t>Count of Start Date</t>
   </si>
+  <si>
+    <t>No se puede cumplir con esta rubrica al ser nuestras variables categoricas</t>
+  </si>
 </sst>
 </file>
 
@@ -501,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -540,6 +544,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,7 +594,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,6 +709,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3881,11 +3897,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3913,7 +3929,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3921,7 +3937,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3937,19 +3953,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$A$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$A$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4429,9 +4445,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4496,9 +4512,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4563,9 +4579,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4630,9 +4646,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4697,9 +4713,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4764,9 +4780,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4831,9 +4847,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4898,9 +4914,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4965,7 +4981,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -5032,9 +5048,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5099,9 +5115,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>215900</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5166,9 +5182,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5233,9 +5249,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5300,9 +5316,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5367,9 +5383,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5434,9 +5450,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5501,9 +5517,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>22</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5568,9 +5584,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5635,9 +5651,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5702,9 +5718,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5769,9 +5785,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
+          <xdr:colOff>371475</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5836,9 +5852,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>31</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5903,9 +5919,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>368300</xdr:colOff>
-          <xdr:row>32</xdr:row>
-          <xdr:rowOff>177800</xdr:rowOff>
+          <xdr:colOff>371475</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6137,6 +6153,10 @@
     </cdr:sp>
   </cdr:relSizeAnchor>
 </c:userShapes>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6980,6 +7000,48 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0E6DE207-A32A-42FE-B495-70664FCE7E90}" name="PivotTable16" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A14:B15" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
+  <pivotFields count="7">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Min of Start Date" fld="3" subtotal="min" baseField="0" baseItem="0"/>
+    <dataField name="Max of Finish Date" fld="4" subtotal="max" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A1D5E49C-13DC-445C-BA4B-79521EEC2B64}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A21:A22" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="7">
@@ -7019,48 +7081,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of Start Date" fld="3" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0E6DE207-A32A-42FE-B495-70664FCE7E90}" name="PivotTable16" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A14:B15" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="7">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Min of Start Date" fld="3" subtotal="min" baseField="0" baseItem="0"/>
-    <dataField name="Max of Finish Date" fld="4" subtotal="max" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -7419,9 +7439,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:PT52"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="15" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="15" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9847,7 +9867,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
@@ -9908,10 +9928,7 @@
       <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="45">
-        <f>Table3[[#This Row],[Start Date]]</f>
-        <v>43952</v>
-      </c>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:9" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
@@ -9937,10 +9954,7 @@
       <c r="G3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="45">
-        <f>E25</f>
-        <v>44002</v>
-      </c>
+      <c r="I3" s="45"/>
     </row>
     <row r="4" spans="1:9" ht="108" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
@@ -9964,10 +9978,6 @@
       </c>
       <c r="G4" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="I4" s="6">
-        <f>I3-I2</f>
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -10489,16 +10499,16 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.90625" style="26" customWidth="1"/>
     <col min="2" max="2" width="36" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.08984375" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.36328125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7265625" style="26" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="26"/>
   </cols>
   <sheetData>
@@ -10527,12 +10537,12 @@
     </row>
     <row r="3" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="49" t="s">
         <v>57</v>
       </c>
       <c r="D3" s="35" t="s">
@@ -10542,7 +10552,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="35" t="s">
         <v>65</v>
@@ -10556,7 +10566,9 @@
       <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="38"/>
+      <c r="A5" s="38" t="b">
+        <v>1</v>
+      </c>
       <c r="B5" s="35" t="s">
         <v>65</v>
       </c>
@@ -10570,7 +10582,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>65</v>
@@ -10584,12 +10596,12 @@
     </row>
     <row r="7" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="49" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="35" t="s">
@@ -10666,7 +10678,9 @@
       <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="A13" s="38"/>
+      <c r="A13" s="38" t="b">
+        <v>1</v>
+      </c>
       <c r="B13" s="35" t="s">
         <v>72</v>
       </c>
@@ -10679,7 +10693,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="35" t="s">
         <v>72</v>
@@ -10698,7 +10712,7 @@
       <c r="B15" s="39"/>
       <c r="C15" s="42">
         <f>COUNTIF(A3:A14, TRUE)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D15" s="40"/>
     </row>
@@ -10751,7 +10765,7 @@
       <c r="B21" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="50" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="35"/>
@@ -10761,7 +10775,7 @@
       <c r="B22" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="50" t="s">
         <v>81</v>
       </c>
       <c r="D22" s="35"/>
@@ -10771,7 +10785,7 @@
       <c r="B23" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="50" t="s">
         <v>82</v>
       </c>
       <c r="D23" s="35"/>
@@ -10781,7 +10795,7 @@
       <c r="B24" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="50" t="s">
         <v>83</v>
       </c>
       <c r="D24" s="35"/>
@@ -10831,7 +10845,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>92</v>
@@ -10841,15 +10855,17 @@
       </c>
       <c r="D30" s="35"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="24" x14ac:dyDescent="0.35">
       <c r="A31" s="38"/>
       <c r="B31" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="35"/>
+      <c r="D31" s="36" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="38" t="b">
@@ -10882,7 +10898,7 @@
       <c r="B34" s="39"/>
       <c r="C34" s="42">
         <f>COUNTIF(A30:A33, TRUE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D34" s="40"/>
     </row>
@@ -11682,6 +11698,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100731F552DF13A6D40B459BD2966D82FC3" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a01b3daf33f8045e07234184d30bca2f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="580b4332-39d2-4436-8fe6-7a9bf13888b4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4ab8cd5de5a730e575350b1bff66377" ns2:_="">
     <xsd:import namespace="580b4332-39d2-4436-8fe6-7a9bf13888b4"/>
@@ -11837,15 +11862,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -11853,6 +11869,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68D788E5-8EC6-49AE-9940-ECDC4AE9184E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F002613-ECC6-485B-9162-F5CCF68EDBA3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11870,14 +11894,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68D788E5-8EC6-49AE-9940-ECDC4AE9184E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8C70C9-4227-49DE-9275-1277DF78A7AB}">
   <ds:schemaRefs>

</xml_diff>